<commit_message>
aggiunto processo perizia e Global.dot
</commit_message>
<xml_diff>
--- a/assessment/assessment.xlsx
+++ b/assessment/assessment.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>PeriziaDaEseguire</t>
+          <t>SelfCareInPerizia</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
@@ -498,7 +498,7 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>SelfCareCompletato</t>
+          <t>SelfCareInChiusura</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -820,12 +820,12 @@
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>DeskCompletata</t>
+          <t>AppuntamentoModificato</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>AvvioPerizia</t>
+          <t>EsecuzioneDesk</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>AppuntamentoModificato</t>
+          <t>AppuntamentoAnnullato</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
@@ -854,7 +854,7 @@
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>AppuntamentoAnnullato</t>
+          <t>DatiObbligatoriMancanti</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
@@ -871,12 +871,12 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>DatiObbligatoriMancanti</t>
+          <t>DeskRifiutata</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneDesk</t>
+          <t>RiassegnazioneDesk</t>
         </is>
       </c>
     </row>
@@ -888,12 +888,12 @@
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>DeskRifiutata</t>
+          <t>DeskCompletata</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>RiassegnazioneDesk</t>
+          <t>AvvioPeriziaPostDesk</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modificati diagrammi opening e assessement
</commit_message>
<xml_diff>
--- a/assessment/assessment.xlsx
+++ b/assessment/assessment.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,9 +563,14 @@
           <t>GestioneSelfCare</t>
         </is>
       </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>AvvioChiusuraPostSelfCare</t>
+        </is>
+      </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>AvvioPerizia</t>
+          <t>AvvioChiusura</t>
         </is>
       </c>
     </row>
@@ -575,14 +580,9 @@
           <t>GestioneSelfCare</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>AvvioChiusuraPostSelfCare</t>
-        </is>
-      </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>AvvioChiusura</t>
+          <t>AvvioPerizia</t>
         </is>
       </c>
     </row>
@@ -628,12 +628,12 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>VisioCompletata</t>
+          <t>VisioCompletataNuovaVisio</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>AvvioPerizia</t>
+          <t>AvvioManualeVisio</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>VisioCompletataNuovaVisio</t>
+          <t>AppuntamentoModificato</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>AvvioManualeVisio</t>
+          <t>EsecuzioneVisio</t>
         </is>
       </c>
     </row>
@@ -662,7 +662,7 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>AppuntamentoModificato</t>
+          <t>AppuntamentoAnnullato</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>AppuntamentoAnnullato</t>
+          <t>DatiObbligatoriMancanti</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
@@ -696,12 +696,12 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>DatiObbligatoriMancanti</t>
+          <t>VisioRifiutata</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneVisio</t>
+          <t>RiassegnazioneVisio</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>VisioRifiutata</t>
+          <t>VisioCompletata</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>RiassegnazioneVisio</t>
+          <t>AvvioPerizia</t>
         </is>
       </c>
     </row>
@@ -742,7 +742,7 @@
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>RichiestaModificaApptoPaVisio</t>
+          <t>Pa_Visio</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -759,7 +759,7 @@
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>ConfermaModificaApptoPaVisio</t>
+          <t>Pa_Visio</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -815,12 +815,12 @@
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>DeskCompletata</t>
+          <t>DeskCompletataNuovaDesk</t>
         </is>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>AvvioPeriziaPostDesk</t>
+          <t>AvvioManualeDesk</t>
         </is>
       </c>
     </row>
@@ -832,12 +832,12 @@
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>DeskCompletataNuovaDesk</t>
+          <t>AppuntamentoModificato</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>AvvioManualeDesk</t>
+          <t>EsecuzioneDesk</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>AppuntamentoModificato</t>
+          <t>AppuntamentoAnnullato</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>AppuntamentoAnnullato</t>
+          <t>DatiObbligatoriMancanti</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
@@ -883,12 +883,12 @@
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>DatiObbligatoriMancanti</t>
+          <t>DeskRifiutata</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneDesk</t>
+          <t>RiassegnazioneDesk</t>
         </is>
       </c>
     </row>
@@ -900,12 +900,12 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>DeskRifiutata</t>
+          <t>DeskCompletata</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>RiassegnazioneDesk</t>
+          <t>AvvioPeriziaPostDesk</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>RichiestaModificaApptoPaDesk</t>
+          <t>Pa_Desk</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
@@ -939,14 +939,14 @@
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneVisio</t>
+          <t>EsecuzioneDesk</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>ConfermaModificaApptoPaDesk</t>
+          <t>Pa_Desk</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneVisio</t>
+          <t>EsecuzioneDesk</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>SoprallugoCompletato</t>
+          <t>AnnullamentoSopralluogo</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>AvvioPerizia</t>
+          <t>AssegnazioneSopralluogo</t>
         </is>
       </c>
     </row>
@@ -1053,12 +1053,12 @@
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>AnnullamentoSopralluogo</t>
+          <t>AppuntamentoAnnullato</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>AssegnazioneSopralluogo</t>
+          <t>PianificazioneSopralluogo</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>AppuntamentoAnnullato</t>
+          <t>ChiusuraAttivita</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>ChiusuraAttivita</t>
+          <t>ChiusuraSoprallVariato</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr">
@@ -1104,12 +1104,12 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>ChiusuraSoprallVariato</t>
+          <t>AppuntamentoModificato</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>PianificazioneSopralluogo</t>
+          <t>EsecuzioneSopralluogo</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>AppuntamentoModificato</t>
+          <t>DatiObbligatoriMancanti</t>
         </is>
       </c>
       <c r="C43" s="2" t="inlineStr">
@@ -1138,12 +1138,12 @@
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>DatiObbligatoriMancanti</t>
+          <t>RichiestaNuovoSopralluogo</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneSopralluogo</t>
+          <t>ApprovazioneSopralluogo</t>
         </is>
       </c>
     </row>
@@ -1155,12 +1155,12 @@
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>SopralluogoCompletatoNuovo</t>
+          <t>AnnullamentoSopralluogo</t>
         </is>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>ApprovazioneSopralluogo</t>
+          <t>AssegnazioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>AvvioSopralluogo</t>
+          <t>PianificazioneSopralluogo</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1218,7 @@
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>RichiestaModificaApptoPaSopralluogo</t>
+          <t>Pa_Sopralluogo</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -1228,14 +1228,14 @@
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneVisio</t>
+          <t>EsecuzioneSopralluogo</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>ConfermaModificaApptoPaSopralluogo</t>
+          <t>Pa_Sopralluogo</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -1245,58 +1245,58 @@
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneVisio</t>
+          <t>EsecuzioneSopralluogo</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>NuovoSopralluogoNonApprovato</t>
+          <t>AvvioSopralluogoPCE</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>NonApprovato</t>
+          <t>SopralluogoAvvioto</t>
         </is>
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>AvvioPerizia</t>
+          <t>AssegnazioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AvvioSopralluogoPCE</t>
+          <t>AssegnazioneSopralluogoPCE</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>SopralluogoPCEAvvioto</t>
+          <t>SopralluogoAssegnato</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>AssegnazioneSopralluogoPCE</t>
+          <t>PianificazioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AssegnazioneSopralluogoPCE</t>
+          <t>PianificazioneSopralluogoPCE</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>SopralluogoPCEAssegnato</t>
+          <t>SopralluogoPianificato</t>
         </is>
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>PianificazioneSopralluogoPCE</t>
+          <t>EsecuzioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
@@ -1308,29 +1308,29 @@
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>SopralluogoPCEPianificato</t>
+          <t>SopralluogoRifiutato</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneSopralluogoPCE</t>
+          <t>VerificaSopralluogoPCEDopoRifiuto</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
+          <t>EsecuzioneSopralluogoPCE</t>
+        </is>
+      </c>
+      <c r="B55" s="2" t="inlineStr">
+        <is>
+          <t>AppuntamentoAnnullato</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="inlineStr">
+        <is>
           <t>PianificazioneSopralluogoPCE</t>
-        </is>
-      </c>
-      <c r="B55" s="2" t="inlineStr">
-        <is>
-          <t>SopralluogoPCERifiutato</t>
-        </is>
-      </c>
-      <c r="C55" s="2" t="inlineStr">
-        <is>
-          <t>VerificaSopralluogoPCEDopoRifiuto</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1342,12 @@
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>SoprallugoCompletato</t>
+          <t>ChiusuraAttivita</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>AvvioPerizia</t>
+          <t>PianificazioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
@@ -1359,12 +1359,12 @@
       </c>
       <c r="B57" s="2" t="inlineStr">
         <is>
-          <t>AnnullamentoSopralluogo</t>
+          <t>ChiusuraSoprallVariato</t>
         </is>
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>AssegnazioneSopralluogoPCE</t>
+          <t>PianificazioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
@@ -1376,12 +1376,12 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>AppuntamentoAnnullato</t>
+          <t>AppuntamentoModificato</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>PianificazioneSopralluogoPCE</t>
+          <t>EsecuzioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
@@ -1393,12 +1393,12 @@
       </c>
       <c r="B59" s="2" t="inlineStr">
         <is>
-          <t>ChiusuraAttivita</t>
+          <t>DatiObbligatoriMancanti</t>
         </is>
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>PianificazioneSopralluogoPCE</t>
+          <t>EsecuzioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
@@ -1410,148 +1410,97 @@
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>ChisuraSoprallVariato</t>
+          <t>RichiestaNuovoSopralluogo</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>PianificazioneSopralluogoPCE</t>
+          <t>ApprovazioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneSopralluogoPCE</t>
+          <t>VerificaSopralluogoPCEDopoRifiuto</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>AppuntamentoModificato</t>
+          <t>SopralluogoAssegnato</t>
         </is>
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneSopralluogoPCE</t>
+          <t>PianificazioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneSopralluogoPCE</t>
+          <t>ApprovazioneSopralluogoPCE</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>DatiObbligatoriMancanti</t>
+          <t>Approvato</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneSopralluogoPCE</t>
+          <t>PianificazioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>EsecuzioneSopralluogoPCE</t>
+          <t>ApprovazioneSopralluogoPCE</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
         <is>
-          <t>SopralluogoPCECompletatoNuovo</t>
+          <t>NonApprovato</t>
         </is>
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>ApprovazioneSopralluogoPCE</t>
+          <t>NuovoSopralluogoNonApprovatoPCE</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>VerificaSopralluogoPCEDopoRifiuto</t>
+          <t>Pa_SopralluogoPCE</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>SopralluogoPCEAssegnato</t>
+          <t>RichiestaPaRicevuta</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>PianificazioneSopralluogoPCE</t>
+          <t>EsecuzioneSopralluogoPCE</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>ApprovazioneSopralluogoPCE</t>
+          <t>Pa_SopralluogoPCE</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
         <is>
-          <t>Approvato</t>
+          <t>ConfermaPaRicevuta</t>
         </is>
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>AvvioSopralluogoPCE</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="2" t="inlineStr">
-        <is>
-          <t>RichiestaModificaApptoPaSopralluogoPCE</t>
-        </is>
-      </c>
-      <c r="B66" s="2" t="inlineStr">
-        <is>
-          <t>RichiestaPaRicevuta</t>
-        </is>
-      </c>
-      <c r="C66" s="2" t="inlineStr">
-        <is>
-          <t>EsecuzioneVisio</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="2" t="inlineStr">
-        <is>
-          <t>ConfermaModificaApptoPaSopralluogoPCE</t>
-        </is>
-      </c>
-      <c r="B67" s="2" t="inlineStr">
-        <is>
-          <t>ConfermaPaRicevuta</t>
-        </is>
-      </c>
-      <c r="C67" s="2" t="inlineStr">
-        <is>
-          <t>EsecuzioneVisio</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="2" t="inlineStr">
-        <is>
-          <t>NuovoSopralluogoNonApprovatoPCE</t>
-        </is>
-      </c>
-      <c r="B68" s="2" t="inlineStr">
-        <is>
-          <t>NonApprovato</t>
-        </is>
-      </c>
-      <c r="C68" s="2" t="inlineStr">
-        <is>
-          <t>AvvioPerizia</t>
+          <t>EsecuzioneSopralluogoPCE</t>
         </is>
       </c>
     </row>

</xml_diff>